<commit_message>
Ghana Jatai runs 19/03/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F559CE-AF96-4EC9-95FE-062A59310409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1942F36-E5F1-4D79-B67A-8ACDF04FBC40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5755" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5763" uniqueCount="1574">
   <si>
     <t>PS</t>
   </si>
@@ -4714,9 +4714,6 @@
   </si>
   <si>
     <t>GRuqtAcI$H ||</t>
-  </si>
-  <si>
-    <t>RE?</t>
   </si>
   <si>
     <t>Table Process</t>
@@ -5360,10 +5357,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1888"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1877" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="Q1673" sqref="Q1673"/>
+      <selection pane="bottomLeft" activeCell="U1888" sqref="U1888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5885,7 +5882,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="T1" s="13" t="s">
         <v>20</v>
@@ -6881,7 +6878,7 @@
         <v>25</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>0</v>
@@ -23786,7 +23783,7 @@
       <c r="S446" s="7"/>
       <c r="T446" s="7"/>
       <c r="U446" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V446" s="21"/>
     </row>
@@ -24120,7 +24117,7 @@
       <c r="S454" s="7"/>
       <c r="T454" s="7"/>
       <c r="U454" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V454" s="21"/>
     </row>
@@ -24966,7 +24963,7 @@
       <c r="S474" s="7"/>
       <c r="T474" s="7"/>
       <c r="U474" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="V474" s="21"/>
     </row>
@@ -26318,7 +26315,7 @@
       <c r="S506" s="7"/>
       <c r="T506" s="7"/>
       <c r="U506" s="7" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="V506" s="21"/>
     </row>
@@ -26440,7 +26437,7 @@
         <v>47</v>
       </c>
       <c r="N509" s="57" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="O509" s="6"/>
       <c r="P509" s="7"/>
@@ -28002,7 +27999,7 @@
         <v>84</v>
       </c>
       <c r="N546" s="21" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="O546" s="6"/>
       <c r="P546" s="7"/>
@@ -28654,7 +28651,7 @@
       <c r="S561" s="7"/>
       <c r="T561" s="7"/>
       <c r="U561" s="7" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="V561" s="21"/>
     </row>
@@ -28697,7 +28694,7 @@
       <c r="S562" s="7"/>
       <c r="T562" s="7"/>
       <c r="U562" s="7" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="V562" s="21"/>
     </row>
@@ -29364,7 +29361,7 @@
       <c r="S578" s="7"/>
       <c r="T578" s="7"/>
       <c r="U578" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="V578" s="21" t="s">
         <v>1440</v>
@@ -30943,7 +30940,7 @@
       <c r="R615" s="7"/>
       <c r="S615" s="7"/>
       <c r="T615" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="U615" s="7"/>
       <c r="V615" s="21" t="s">
@@ -31448,7 +31445,7 @@
       <c r="S627" s="7"/>
       <c r="T627" s="7"/>
       <c r="U627" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="V627" s="21"/>
     </row>
@@ -31995,7 +31992,7 @@
       <c r="S640" s="7"/>
       <c r="T640" s="7"/>
       <c r="U640" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V640" s="21"/>
     </row>
@@ -32626,7 +32623,7 @@
       <c r="S655" s="7"/>
       <c r="T655" s="7"/>
       <c r="U655" s="7" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="V655" s="21"/>
     </row>
@@ -33491,7 +33488,7 @@
       <c r="S675" s="7"/>
       <c r="T675" s="7"/>
       <c r="U675" s="7" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="V675" s="21"/>
     </row>
@@ -35331,7 +35328,7 @@
       <c r="S718" s="7"/>
       <c r="T718" s="7"/>
       <c r="U718" s="7" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="V718" s="21"/>
     </row>
@@ -36154,7 +36151,7 @@
       <c r="S737" s="7"/>
       <c r="T737" s="7"/>
       <c r="U737" s="7" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="V737" s="21"/>
     </row>
@@ -36329,7 +36326,7 @@
         <v>1514</v>
       </c>
       <c r="T741" s="7" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="U741" s="7"/>
       <c r="V741" s="21"/>
@@ -37331,7 +37328,7 @@
         <v>1514</v>
       </c>
       <c r="T764" s="7" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="U764" s="7"/>
       <c r="V764" s="21"/>
@@ -38239,7 +38236,7 @@
       <c r="S785" s="7"/>
       <c r="T785" s="7"/>
       <c r="U785" s="7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="V785" s="21"/>
     </row>
@@ -38712,7 +38709,7 @@
       <c r="S796" s="7"/>
       <c r="T796" s="7"/>
       <c r="U796" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V796" s="21"/>
     </row>
@@ -39263,7 +39260,7 @@
       <c r="S809" s="7"/>
       <c r="T809" s="7"/>
       <c r="U809" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V809" s="21"/>
     </row>
@@ -39390,7 +39387,7 @@
       <c r="S812" s="7"/>
       <c r="T812" s="7"/>
       <c r="U812" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V812" s="21"/>
     </row>
@@ -40863,7 +40860,7 @@
       <c r="S846" s="7"/>
       <c r="T846" s="7"/>
       <c r="U846" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V846" s="21" t="s">
         <v>1471</v>
@@ -58967,7 +58964,7 @@
         <v>1514</v>
       </c>
       <c r="T1294" s="7" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="U1294" s="7"/>
       <c r="V1294" s="21"/>
@@ -69142,7 +69139,7 @@
       <c r="S1552" s="7"/>
       <c r="T1552" s="7"/>
       <c r="U1552" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1552" s="21"/>
     </row>
@@ -69253,7 +69250,7 @@
       <c r="S1555" s="7"/>
       <c r="T1555" s="7"/>
       <c r="U1555" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1555" s="21"/>
     </row>
@@ -69364,7 +69361,7 @@
       <c r="S1558" s="7"/>
       <c r="T1558" s="7"/>
       <c r="U1558" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1558" s="21"/>
     </row>
@@ -69475,7 +69472,7 @@
       <c r="S1561" s="7"/>
       <c r="T1561" s="7"/>
       <c r="U1561" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1561" s="21"/>
     </row>
@@ -69722,7 +69719,7 @@
       <c r="S1568" s="7"/>
       <c r="T1568" s="7"/>
       <c r="U1568" s="7" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1568" s="21"/>
     </row>
@@ -70583,7 +70580,7 @@
         <v>328</v>
       </c>
       <c r="U1598" s="1" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1598" s="21"/>
     </row>
@@ -71031,7 +71028,7 @@
         <v>328</v>
       </c>
       <c r="U1615" s="1" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1615" s="21"/>
     </row>
@@ -71671,7 +71668,7 @@
         <v>960</v>
       </c>
       <c r="U1638" s="1" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="V1638" s="21"/>
     </row>
@@ -72166,7 +72163,7 @@
         <v>971</v>
       </c>
       <c r="U1655" s="1" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="V1655" s="21"/>
     </row>
@@ -72508,7 +72505,7 @@
         <v>976</v>
       </c>
       <c r="U1667" s="1" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="V1667" s="21"/>
     </row>
@@ -73654,6 +73651,9 @@
       <c r="N1707" s="21" t="s">
         <v>648</v>
       </c>
+      <c r="U1707" s="1" t="s">
+        <v>1531</v>
+      </c>
       <c r="V1707" s="21"/>
     </row>
     <row r="1708" spans="3:22" x14ac:dyDescent="0.25">
@@ -74533,6 +74533,9 @@
       <c r="N1738" s="21" t="s">
         <v>648</v>
       </c>
+      <c r="U1738" s="1" t="s">
+        <v>1531</v>
+      </c>
       <c r="V1738" s="21"/>
     </row>
     <row r="1739" spans="3:22" x14ac:dyDescent="0.25">
@@ -74916,6 +74919,9 @@
       <c r="O1751" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="U1751" s="1" t="s">
+        <v>1531</v>
+      </c>
       <c r="V1751" s="21"/>
     </row>
     <row r="1752" spans="3:22" x14ac:dyDescent="0.25">
@@ -75770,9 +75776,6 @@
       <c r="N1780" s="21" t="s">
         <v>1042</v>
       </c>
-      <c r="U1780" s="1" t="s">
-        <v>1562</v>
-      </c>
       <c r="V1780" s="21"/>
     </row>
     <row r="1781" spans="3:22" x14ac:dyDescent="0.25">
@@ -76047,9 +76050,6 @@
       <c r="N1789" s="21" t="s">
         <v>1047</v>
       </c>
-      <c r="U1789" s="1" t="s">
-        <v>1562</v>
-      </c>
       <c r="V1789" s="21"/>
     </row>
     <row r="1790" spans="3:22" x14ac:dyDescent="0.25">
@@ -76639,6 +76639,9 @@
       <c r="P1809" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="U1809" s="1" t="s">
+        <v>1564</v>
+      </c>
       <c r="V1809" s="21" t="s">
         <v>1494</v>
       </c>
@@ -76915,6 +76918,9 @@
       <c r="P1818" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="U1818" s="1" t="s">
+        <v>1564</v>
+      </c>
       <c r="V1818" s="21" t="s">
         <v>1475</v>
       </c>
@@ -77065,6 +77071,9 @@
       <c r="O1823" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="U1823" s="1" t="s">
+        <v>1573</v>
+      </c>
       <c r="V1823" s="21"/>
     </row>
     <row r="1824" spans="3:22" x14ac:dyDescent="0.25">
@@ -77367,6 +77376,9 @@
       <c r="P1833" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="U1833" s="1" t="s">
+        <v>1564</v>
+      </c>
       <c r="V1833" s="21" t="s">
         <v>1475</v>
       </c>
@@ -77769,13 +77781,13 @@
         <f t="shared" si="86"/>
         <v>223</v>
       </c>
-      <c r="N1847" s="21" t="s">
+      <c r="N1847" s="57" t="s">
         <v>1152</v>
       </c>
       <c r="O1847" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V1847" s="21" t="s">
+      <c r="V1847" s="57" t="s">
         <v>1078</v>
       </c>
     </row>
@@ -78297,6 +78309,9 @@
       <c r="N1865" s="21" t="s">
         <v>648</v>
       </c>
+      <c r="U1865" s="1" t="s">
+        <v>1564</v>
+      </c>
       <c r="V1865" s="21"/>
     </row>
     <row r="1866" spans="3:22" x14ac:dyDescent="0.25">
@@ -78324,6 +78339,9 @@
       <c r="N1866" s="21" t="s">
         <v>794</v>
       </c>
+      <c r="U1866" s="1" t="s">
+        <v>1531</v>
+      </c>
       <c r="V1866" s="21"/>
     </row>
     <row r="1867" spans="3:22" x14ac:dyDescent="0.25">
@@ -78959,6 +78977,9 @@
       </c>
       <c r="N1887" s="21" t="s">
         <v>541</v>
+      </c>
+      <c r="U1887" s="1" t="s">
+        <v>1564</v>
       </c>
       <c r="V1887" s="21"/>
     </row>

</xml_diff>